<commit_message>
Añade correcciones para Cobros Anticipo, Cobros, SAldos cliente y Devoluciones fact Ant
</commit_message>
<xml_diff>
--- a/Correcciones/Saldos Cte/PolizaSaldosCte_IVA.xlsx
+++ b/Correcciones/Saldos Cte/PolizaSaldosCte_IVA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -100,16 +100,16 @@
     <t>Cxc.Sucursal</t>
   </si>
   <si>
+    <t>'217-250-000-0000'</t>
+  </si>
+  <si>
     <t>Cxc.Impuestos</t>
   </si>
   <si>
-    <t>'700-560-000-0000'</t>
-  </si>
-  <si>
     <t>Cxc.Importe</t>
   </si>
   <si>
-    <t>217-250-000-0000'</t>
+    <t>700-560-000-0000'</t>
   </si>
 </sst>
 </file>
@@ -161,7 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +445,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,8 +578,8 @@
       <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>25</v>
+      <c r="E3" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F3" t="s">
         <v>21</v>
@@ -634,8 +634,8 @@
       <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>27</v>
+      <c r="E4" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>21</v>
@@ -644,7 +644,7 @@
         <v>21</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>21</v>

</xml_diff>